<commit_message>
fixed a few bugs. update reference simulation
</commit_message>
<xml_diff>
--- a/variables_SUREAU-ECOS.xlsx
+++ b/variables_SUREAU-ECOS.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jruffault/Dropbox/Mon Mac (MacBook-Pro-de-Julien.local)/Desktop/SurEau-Ecos_V4.0/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5CA8C2DE-F7E2-0D45-B3D5-46841CE0585C}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F4E7868C-2CB3-9C4A-B41D-A661E4EE1BD6}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="10260" yWindow="4100" windowWidth="27640" windowHeight="16540" xr2:uid="{786E4E24-E824-9545-940F-9376694D6E3F}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="94" uniqueCount="88">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="88" uniqueCount="83">
   <si>
     <t>Name</t>
   </si>
@@ -129,15 +129,6 @@
     <t>kAllSoilToCollar</t>
   </si>
   <si>
-    <t>KAllSoilToCanopy</t>
-  </si>
-  <si>
-    <t>kAboveGround</t>
-  </si>
-  <si>
-    <t>kBelowGround</t>
-  </si>
-  <si>
     <t>kRoot2</t>
   </si>
   <si>
@@ -169,12 +160,6 @@
   </si>
   <si>
     <t>sum of kSoil to Collar</t>
-  </si>
-  <si>
-    <t>?</t>
-  </si>
-  <si>
-    <t xml:space="preserve">deppreciated </t>
   </si>
   <si>
     <t xml:space="preserve">Symplasmic leaf capacitance </t>
@@ -295,17 +280,10 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="12"/>
-      <color rgb="FFFF0000"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -319,7 +297,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -329,12 +307,6 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFFFFF00"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.79998168889431442"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -351,10 +323,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
@@ -670,10 +641,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{62BE3869-25F7-9A46-B413-E7E0C8AEB262}">
-  <dimension ref="A1:C66"/>
+  <dimension ref="A1:C63"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A5" zoomScale="233" workbookViewId="0">
-      <selection activeCell="A55" sqref="A55"/>
+    <sheetView tabSelected="1" zoomScale="233" workbookViewId="0">
+      <selection activeCell="A5" sqref="A5:XFD5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -714,102 +685,99 @@
         <v>33</v>
       </c>
       <c r="B5" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A7" t="s">
         <v>34</v>
       </c>
-      <c r="B6" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A7" s="2" t="s">
-        <v>35</v>
-      </c>
-      <c r="B7" s="2" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="8" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A8" s="2" t="s">
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A8" t="s">
         <v>36</v>
-      </c>
-      <c r="B8" s="2" t="s">
-        <v>49</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>39</v>
       </c>
+      <c r="B11" t="s">
+        <v>45</v>
+      </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>40</v>
       </c>
+      <c r="B12" t="s">
+        <v>46</v>
+      </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>41</v>
       </c>
+      <c r="B13" t="s">
+        <v>47</v>
+      </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>42</v>
       </c>
       <c r="B14" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A15" s="2" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A16" s="2" t="s">
         <v>50</v>
-      </c>
-    </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A15" t="s">
-        <v>43</v>
-      </c>
-      <c r="B15" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A16" t="s">
-        <v>44</v>
-      </c>
-      <c r="B16" t="s">
-        <v>52</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
-        <v>45</v>
-      </c>
-      <c r="B17" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A18" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A19" t="s">
         <v>53</v>
-      </c>
-    </row>
-    <row r="18" spans="1:3" s="3" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A18" s="3" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="19" spans="1:3" s="3" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A19" s="3" t="s">
-        <v>55</v>
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
+        <v>54</v>
+      </c>
+      <c r="B20" t="s">
+        <v>55</v>
+      </c>
+      <c r="C20" t="s">
         <v>56</v>
       </c>
     </row>
@@ -817,284 +785,263 @@
       <c r="A21" t="s">
         <v>57</v>
       </c>
+      <c r="B21" t="s">
+        <v>58</v>
+      </c>
+      <c r="C21" t="s">
+        <v>56</v>
+      </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
-        <v>58</v>
+        <v>3</v>
+      </c>
+      <c r="B22" t="s">
+        <v>59</v>
+      </c>
+      <c r="C22" t="s">
+        <v>56</v>
       </c>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
-        <v>59</v>
+        <v>4</v>
       </c>
       <c r="B23" t="s">
         <v>60</v>
       </c>
       <c r="C23" t="s">
-        <v>61</v>
+        <v>56</v>
       </c>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
-        <v>62</v>
-      </c>
-      <c r="B24" t="s">
-        <v>63</v>
-      </c>
-      <c r="C24" t="s">
-        <v>61</v>
+        <v>5</v>
       </c>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
-        <v>3</v>
-      </c>
-      <c r="B25" t="s">
-        <v>64</v>
-      </c>
-      <c r="C25" t="s">
-        <v>61</v>
+        <v>6</v>
       </c>
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
-        <v>4</v>
-      </c>
-      <c r="B26" t="s">
-        <v>65</v>
-      </c>
-      <c r="C26" t="s">
-        <v>61</v>
+        <v>7</v>
       </c>
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
-        <v>5</v>
+        <v>8</v>
       </c>
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
-        <v>6</v>
+        <v>9</v>
       </c>
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
-        <v>7</v>
+        <v>10</v>
       </c>
     </row>
     <row r="30" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
-        <v>8</v>
+        <v>11</v>
       </c>
     </row>
     <row r="31" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
-        <v>9</v>
+        <v>12</v>
       </c>
     </row>
     <row r="32" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
-        <v>10</v>
+        <v>13</v>
       </c>
     </row>
     <row r="33" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
-        <v>11</v>
+        <v>14</v>
       </c>
     </row>
     <row r="34" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
-        <v>12</v>
+        <v>15</v>
       </c>
     </row>
     <row r="35" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
-        <v>13</v>
+        <v>16</v>
       </c>
     </row>
     <row r="36" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
     </row>
     <row r="37" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
-        <v>15</v>
+        <v>18</v>
       </c>
     </row>
     <row r="38" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A38" t="s">
-        <v>16</v>
+        <v>19</v>
       </c>
     </row>
     <row r="39" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A39" t="s">
-        <v>17</v>
+        <v>20</v>
       </c>
     </row>
     <row r="40" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A40" t="s">
-        <v>18</v>
+        <v>21</v>
       </c>
     </row>
     <row r="41" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A41" t="s">
-        <v>19</v>
+        <v>22</v>
       </c>
     </row>
     <row r="42" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A42" t="s">
-        <v>20</v>
+        <v>23</v>
       </c>
     </row>
     <row r="43" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A43" t="s">
-        <v>21</v>
+        <v>24</v>
       </c>
     </row>
     <row r="44" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A44" t="s">
-        <v>22</v>
+        <v>25</v>
       </c>
     </row>
     <row r="45" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A45" t="s">
-        <v>23</v>
+        <v>26</v>
       </c>
     </row>
     <row r="46" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A46" t="s">
-        <v>24</v>
+        <v>27</v>
       </c>
     </row>
     <row r="47" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A47" t="s">
-        <v>25</v>
+        <v>28</v>
       </c>
     </row>
     <row r="48" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A48" t="s">
-        <v>26</v>
+        <v>29</v>
       </c>
     </row>
     <row r="49" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A49" t="s">
-        <v>27</v>
+        <v>80</v>
       </c>
     </row>
     <row r="50" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A50" t="s">
-        <v>28</v>
+        <v>81</v>
       </c>
     </row>
     <row r="51" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A51" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="52" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A52" t="s">
-        <v>85</v>
+        <v>82</v>
+      </c>
+    </row>
+    <row r="52" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A52" s="2" t="s">
+        <v>79</v>
       </c>
     </row>
     <row r="53" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A53" t="s">
-        <v>86</v>
+        <v>78</v>
+      </c>
+      <c r="B53" t="s">
+        <v>73</v>
+      </c>
+      <c r="C53" t="s">
+        <v>74</v>
       </c>
     </row>
     <row r="54" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A54" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="55" spans="1:3" s="3" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A55" s="3" t="s">
-        <v>84</v>
+        <v>70</v>
+      </c>
+      <c r="B54" t="s">
+        <v>71</v>
+      </c>
+      <c r="C54" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="55" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A55" t="s">
+        <v>69</v>
       </c>
     </row>
     <row r="56" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A56" t="s">
-        <v>83</v>
+        <v>77</v>
       </c>
       <c r="B56" t="s">
-        <v>78</v>
+        <v>68</v>
       </c>
       <c r="C56" t="s">
-        <v>79</v>
+        <v>66</v>
       </c>
     </row>
     <row r="57" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A57" t="s">
-        <v>75</v>
+        <v>65</v>
       </c>
       <c r="B57" t="s">
-        <v>76</v>
+        <v>67</v>
       </c>
       <c r="C57" t="s">
-        <v>77</v>
+        <v>66</v>
       </c>
     </row>
     <row r="58" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A58" t="s">
-        <v>74</v>
+        <v>76</v>
+      </c>
+      <c r="B58" t="s">
+        <v>75</v>
+      </c>
+      <c r="C58" t="s">
+        <v>66</v>
       </c>
     </row>
     <row r="59" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A59" t="s">
-        <v>82</v>
-      </c>
-      <c r="B59" t="s">
-        <v>73</v>
-      </c>
-      <c r="C59" t="s">
-        <v>71</v>
+        <v>64</v>
       </c>
     </row>
     <row r="60" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A60" t="s">
-        <v>70</v>
-      </c>
-      <c r="B60" t="s">
-        <v>72</v>
-      </c>
-      <c r="C60" t="s">
-        <v>71</v>
+        <v>63</v>
       </c>
     </row>
     <row r="61" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A61" t="s">
-        <v>81</v>
-      </c>
-      <c r="B61" t="s">
-        <v>80</v>
-      </c>
-      <c r="C61" t="s">
-        <v>71</v>
+        <v>62</v>
       </c>
     </row>
     <row r="62" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A62" t="s">
-        <v>69</v>
+        <v>61</v>
       </c>
     </row>
     <row r="63" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A63" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="64" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A64" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="65" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A65" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="66" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A66" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
     </row>
   </sheetData>

</xml_diff>